<commit_message>
Added construction images and updated some hardware items in the spreadsheet
</commit_message>
<xml_diff>
--- a/hardware/hardware_spreadsheet_not_campbellsci.xlsx
+++ b/hardware/hardware_spreadsheet_not_campbellsci.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedon Dority\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedon Dority\Documents\GitHub\snow_sensing\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4E44AC57-65DE-495F-A164-4ED74986E98D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1158E525-C63E-4500-9CC9-AE1EC3E9C686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{6EB52CEB-1D4B-9D4B-8914-58F1C62D238A}"/>
+    <workbookView xWindow="25490" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{6EB52CEB-1D4B-9D4B-8914-58F1C62D238A}"/>
   </bookViews>
   <sheets>
     <sheet name="Low-Cost Snow Station" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="114">
   <si>
     <t>Item</t>
   </si>
@@ -329,15 +329,9 @@
     <t xml:space="preserve">For fastening the enclosure to the mast and for the solar panel. For the solar panel, you may want to get a u-bolt with a plate. These are zinc plated. Stainless would be better but more expensive. You may also have better luck finding them at Lowes or Campbell Scientific. </t>
   </si>
   <si>
-    <t xml:space="preserve">    Nuts</t>
-  </si>
-  <si>
     <t>For improving the solar panel mount's rigidity</t>
   </si>
   <si>
-    <t xml:space="preserve">    Bolts</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Grounding rod and wire clamp</t>
   </si>
   <si>
@@ -405,6 +399,9 @@
   </si>
   <si>
     <t>Only necessary if locating solar panel away from station, in which case you will need to measure out how much you need.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    Nuts and bolts</t>
   </si>
 </sst>
 </file>
@@ -489,7 +486,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -505,13 +502,10 @@
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="6" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="3"/>
-    <xf numFmtId="6" fontId="4" fillId="3" borderId="0" xfId="3" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -829,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4E0150-E134-1049-A012-C7D00DAA06DE}">
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1000,7 +994,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B10">
         <v>1</v>
@@ -1021,7 +1015,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -1042,7 +1036,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -1063,7 +1057,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B13">
         <v>1</v>
@@ -1084,7 +1078,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B14">
         <v>1</v>
@@ -1126,7 +1120,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -1147,7 +1141,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -1227,7 +1221,7 @@
       <c r="B23">
         <v>4</v>
       </c>
-      <c r="C23" s="16">
+      <c r="C23" s="15">
         <v>2.08</v>
       </c>
       <c r="D23" s="7">
@@ -1243,7 +1237,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B24">
         <v>2</v>
@@ -1252,7 +1246,7 @@
         <v>42</v>
       </c>
       <c r="D24" s="7">
-        <f t="shared" ref="D24:D25" si="2">B24*C24</f>
+        <f t="shared" ref="D24" si="2">B24*C24</f>
         <v>84</v>
       </c>
       <c r="E24" s="6" t="s">
@@ -1264,7 +1258,7 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B25">
         <v>2</v>
@@ -1281,544 +1275,565 @@
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="20" t="s">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" s="7">
+        <v>1.48</v>
+      </c>
+      <c r="D26" s="7">
+        <f>C26*B26</f>
+        <v>1.48</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" t="s">
         <v>89</v>
       </c>
-      <c r="B26" s="20">
-        <v>2</v>
-      </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="21"/>
-      <c r="F26" s="20" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="20" t="s">
-        <v>97</v>
-      </c>
-      <c r="B27" s="20">
-        <v>1</v>
-      </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="21"/>
-      <c r="F27" s="20" t="s">
-        <v>98</v>
+      <c r="A27" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>11.89</v>
+      </c>
+      <c r="D27">
+        <f>C27*B27</f>
+        <v>11.89</v>
+      </c>
+      <c r="E27" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B28" s="20">
-        <v>2</v>
-      </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="21"/>
-      <c r="F28" s="20" t="s">
-        <v>90</v>
+      <c r="A28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" s="7">
+        <v>3.43</v>
+      </c>
+      <c r="D28" s="7">
+        <f t="shared" ref="D28:D35" si="3">B28*C28</f>
+        <v>3.43</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>84</v>
       </c>
       <c r="B29">
         <v>1</v>
       </c>
       <c r="C29" s="7">
-        <v>3.43</v>
+        <v>9.98</v>
       </c>
       <c r="D29" s="7">
-        <f t="shared" ref="D29:D36" si="3">B29*C29</f>
-        <v>3.43</v>
+        <f t="shared" si="3"/>
+        <v>9.98</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F29" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>35</v>
       </c>
       <c r="B30">
         <v>1</v>
       </c>
       <c r="C30" s="7">
-        <v>9.98</v>
+        <v>7.4</v>
       </c>
       <c r="D30" s="7">
         <f t="shared" si="3"/>
-        <v>9.98</v>
+        <v>7.4</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F30" t="s">
-        <v>85</v>
+        <v>52</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>66</v>
       </c>
       <c r="B31">
         <v>1</v>
       </c>
       <c r="C31" s="7">
-        <v>7.4</v>
+        <v>8.49</v>
       </c>
       <c r="D31" s="7">
         <f t="shared" si="3"/>
-        <v>7.4</v>
+        <v>8.49</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F31" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B32">
         <v>1</v>
       </c>
       <c r="C32" s="7">
-        <v>8.49</v>
+        <v>54.99</v>
       </c>
       <c r="D32" s="7">
         <f t="shared" si="3"/>
-        <v>8.49</v>
+        <v>54.99</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F32" t="s">
-        <v>53</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B33">
         <v>1</v>
       </c>
       <c r="C33" s="7">
-        <v>54.99</v>
+        <v>7.49</v>
       </c>
       <c r="D33" s="7">
         <f t="shared" si="3"/>
-        <v>54.99</v>
+        <v>7.49</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F33" t="s">
-        <v>69</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="B34">
         <v>1</v>
       </c>
       <c r="C34" s="7">
-        <v>7.49</v>
+        <v>4.68</v>
       </c>
       <c r="D34" s="7">
         <f t="shared" si="3"/>
-        <v>7.49</v>
+        <v>4.68</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F34" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>43</v>
+        <v>107</v>
       </c>
       <c r="B35">
         <v>1</v>
       </c>
       <c r="C35" s="7">
-        <v>4.68</v>
+        <v>103</v>
       </c>
       <c r="D35" s="7">
         <f t="shared" si="3"/>
-        <v>4.68</v>
+        <v>103</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F35" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>109</v>
-      </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" s="7">
-        <v>103</v>
-      </c>
-      <c r="D36" s="7">
-        <f t="shared" si="3"/>
-        <v>103</v>
-      </c>
-      <c r="E36" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="s">
+      <c r="A36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D37" s="8">
-        <f>SUM(D22:D36)</f>
-        <v>569.76</v>
-      </c>
-      <c r="E37" s="5"/>
+      <c r="D36" s="8">
+        <f>SUM(D22:D35)</f>
+        <v>583.13000000000011</v>
+      </c>
+      <c r="E36" s="5"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F38" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>5</v>
+        <v>64</v>
+      </c>
+      <c r="B39">
+        <v>1</v>
+      </c>
+      <c r="C39" s="7">
+        <v>7.6</v>
+      </c>
+      <c r="D39" s="7">
+        <f>B39*C39</f>
+        <v>7.6</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F39" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>64</v>
+      <c r="A40" t="s">
+        <v>70</v>
       </c>
       <c r="B40">
         <v>1</v>
       </c>
-      <c r="C40" s="7">
-        <v>7.6</v>
+      <c r="C40">
+        <v>74.989999999999995</v>
       </c>
       <c r="D40" s="7">
-        <f>B40*C40</f>
-        <v>7.6</v>
-      </c>
-      <c r="E40" s="3" t="s">
+        <f t="shared" ref="D40:D44" si="4">B40*C40</f>
+        <v>74.989999999999995</v>
+      </c>
+      <c r="E40" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F40" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>70</v>
+        <v>108</v>
       </c>
       <c r="B41">
         <v>1</v>
       </c>
       <c r="C41">
-        <v>74.989999999999995</v>
+        <v>9.99</v>
       </c>
       <c r="D41" s="7">
-        <f t="shared" ref="D41:D45" si="4">B41*C41</f>
-        <v>74.989999999999995</v>
+        <f>B41*C41</f>
+        <v>9.99</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F41" t="s">
-        <v>71</v>
+        <v>87</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B42">
         <v>1</v>
       </c>
-      <c r="C42">
-        <v>9.99</v>
+      <c r="C42" s="7">
+        <v>7.54</v>
       </c>
       <c r="D42" s="7">
         <f>B42*C42</f>
-        <v>9.99</v>
+        <v>7.54</v>
       </c>
       <c r="E42" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F42" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B43">
         <v>1</v>
       </c>
       <c r="C43" s="7">
-        <v>7.54</v>
+        <v>6.63</v>
       </c>
       <c r="D43" s="7">
         <f>B43*C43</f>
-        <v>7.54</v>
+        <v>6.63</v>
       </c>
       <c r="E43" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F43" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>112</v>
+        <v>72</v>
       </c>
       <c r="B44">
         <v>1</v>
       </c>
       <c r="C44" s="7">
-        <v>6.63</v>
+        <v>86.99</v>
       </c>
       <c r="D44" s="7">
-        <f>B44*C44</f>
-        <v>6.63</v>
+        <f t="shared" si="4"/>
+        <v>86.99</v>
       </c>
       <c r="E44" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F44" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B45">
         <v>1</v>
       </c>
-      <c r="C45" s="7">
-        <v>86.99</v>
+      <c r="C45" s="15">
+        <v>8.99</v>
       </c>
       <c r="D45" s="7">
-        <f t="shared" si="4"/>
-        <v>86.99</v>
+        <f t="shared" ref="D45:D49" si="5">B45*C45</f>
+        <v>8.99</v>
       </c>
       <c r="E45" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>67</v>
+        <v>91</v>
       </c>
       <c r="B46">
-        <v>1</v>
-      </c>
-      <c r="C46" s="16">
-        <v>8.99</v>
+        <v>4</v>
+      </c>
+      <c r="C46" s="15">
+        <v>1.98</v>
       </c>
       <c r="D46" s="7">
-        <f t="shared" ref="D46:D50" si="5">B46*C46</f>
-        <v>8.99</v>
+        <f t="shared" si="5"/>
+        <v>7.92</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F46" t="s">
-        <v>74</v>
+        <v>92</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B47">
-        <v>4</v>
-      </c>
-      <c r="C47" s="16">
-        <v>1.98</v>
+        <v>1</v>
+      </c>
+      <c r="C47" s="15">
+        <v>19.7</v>
       </c>
       <c r="D47" s="7">
         <f t="shared" si="5"/>
-        <v>7.92</v>
+        <v>19.7</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="F47" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
-      <c r="C48" s="16">
-        <v>19.7</v>
+      <c r="C48" s="15">
+        <v>8.98</v>
       </c>
       <c r="D48" s="7">
         <f t="shared" si="5"/>
-        <v>19.7</v>
+        <v>8.98</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>16</v>
+      </c>
+      <c r="F48" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>111</v>
       </c>
       <c r="B49">
         <v>1</v>
       </c>
-      <c r="C49" s="16">
-        <v>8.98</v>
+      <c r="C49" s="15">
+        <v>15.5</v>
       </c>
       <c r="D49" s="7">
         <f t="shared" si="5"/>
-        <v>8.98</v>
+        <v>15.5</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F49" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>113</v>
-      </c>
-      <c r="B50">
-        <v>1</v>
-      </c>
-      <c r="C50" s="16">
-        <v>15.5</v>
-      </c>
-      <c r="D50" s="7">
-        <f t="shared" si="5"/>
-        <v>15.5</v>
-      </c>
-      <c r="E50" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F50" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="s">
+      <c r="A50" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="8">
-        <f>SUM(D40:D50)</f>
+      <c r="B50" s="2"/>
+      <c r="C50" s="8"/>
+      <c r="D50" s="8">
+        <f>SUM(D39:D49)</f>
         <v>254.82999999999996</v>
       </c>
-      <c r="E51" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A52" s="2" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A53" s="2" t="s">
-        <v>4</v>
+      <c r="A53" t="s">
+        <v>22</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53" s="7">
+        <v>258</v>
+      </c>
+      <c r="D53" s="7">
+        <f t="shared" ref="D53:D59" si="6">B53*C53</f>
+        <v>774</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F53" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>22</v>
+        <v>62</v>
       </c>
       <c r="B54">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C54" s="7">
-        <v>258</v>
+        <v>134</v>
       </c>
       <c r="D54" s="7">
-        <f t="shared" ref="D54:D60" si="6">B54*C54</f>
-        <v>774</v>
-      </c>
-      <c r="E54" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A55" t="s">
-        <v>62</v>
-      </c>
-      <c r="B55">
-        <v>1</v>
-      </c>
-      <c r="C55" s="7">
-        <v>134</v>
-      </c>
-      <c r="D55" s="7">
         <f t="shared" si="6"/>
         <v>134</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" t="s">
+      <c r="E54" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A56" s="17" t="s">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A55" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B56" s="17">
+      <c r="B55" s="16">
         <v>10</v>
       </c>
-      <c r="C56" s="18">
+      <c r="C55" s="17">
         <v>0.59</v>
       </c>
-      <c r="D56" s="18">
+      <c r="D55" s="17">
         <f t="shared" si="6"/>
         <v>5.8999999999999995</v>
       </c>
-      <c r="E56" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F56" s="17" t="s">
+      <c r="E55" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="16" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56">
+        <v>1</v>
+      </c>
+      <c r="C56" s="7">
+        <v>599</v>
+      </c>
+      <c r="D56" s="7">
+        <f t="shared" si="6"/>
+        <v>599</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B57">
         <v>1</v>
@@ -1830,228 +1845,207 @@
         <f t="shared" si="6"/>
         <v>599</v>
       </c>
-      <c r="E57" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F57" s="7" t="s">
+      <c r="E57" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F57" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B58">
         <v>1</v>
       </c>
       <c r="C58" s="7">
-        <v>599</v>
+        <v>663</v>
       </c>
       <c r="D58" s="7">
         <f t="shared" si="6"/>
-        <v>599</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F58" t="s">
+        <v>663</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F58" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="B59">
         <v>1</v>
       </c>
       <c r="C59" s="7">
-        <v>663</v>
+        <v>85</v>
       </c>
       <c r="D59" s="7">
         <f t="shared" si="6"/>
-        <v>663</v>
+        <v>85</v>
       </c>
       <c r="E59" s="4" t="s">
         <v>16</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>37</v>
+        <v>76</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A60" t="s">
-        <v>75</v>
-      </c>
-      <c r="B60">
-        <v>1</v>
-      </c>
-      <c r="C60" s="7">
-        <v>85</v>
-      </c>
-      <c r="D60" s="7">
-        <f t="shared" si="6"/>
-        <v>85</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>76</v>
-      </c>
+      <c r="A60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" s="2"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="8">
+        <f>SUM(D53:D59)</f>
+        <v>2859.9</v>
+      </c>
+      <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A61" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B61" s="2"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="8">
-        <f>SUM(D54:D60)</f>
-        <v>2859.9</v>
-      </c>
-      <c r="E61" s="5"/>
+      <c r="E61" s="1"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A62" s="2" t="s">
+        <v>33</v>
+      </c>
       <c r="E62" s="1"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E63" s="1"/>
+      <c r="A63" t="s">
+        <v>77</v>
+      </c>
+      <c r="B63">
+        <v>1</v>
+      </c>
+      <c r="C63" s="15">
+        <v>52</v>
+      </c>
+      <c r="D63" s="7">
+        <f t="shared" ref="D63:D66" si="7">B63*C63</f>
+        <v>52</v>
+      </c>
+      <c r="E63" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F63" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B64">
         <v>1</v>
       </c>
-      <c r="C64" s="16">
-        <v>52</v>
+      <c r="C64" s="15">
+        <v>28.77</v>
       </c>
       <c r="D64" s="7">
-        <f t="shared" ref="D64:D67" si="7">B64*C64</f>
-        <v>52</v>
+        <f>B64*C64</f>
+        <v>28.77</v>
       </c>
       <c r="E64" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F64" t="s">
-        <v>60</v>
+        <v>81</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A65" t="s">
-        <v>80</v>
+      <c r="A65" s="2" t="s">
+        <v>78</v>
       </c>
       <c r="B65">
         <v>1</v>
       </c>
-      <c r="C65" s="16">
-        <v>28.77</v>
+      <c r="C65" s="15">
+        <v>5.98</v>
       </c>
       <c r="D65" s="7">
         <f>B65*C65</f>
-        <v>28.77</v>
+        <v>5.98</v>
       </c>
       <c r="E65" s="6" t="s">
         <v>16</v>
       </c>
       <c r="F65" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A66" s="2" t="s">
-        <v>78</v>
+      <c r="A66" t="s">
+        <v>59</v>
       </c>
       <c r="B66">
         <v>1</v>
       </c>
-      <c r="C66" s="16">
-        <v>5.98</v>
+      <c r="C66" s="15">
+        <v>162.24</v>
       </c>
       <c r="D66" s="7">
-        <f>B66*C66</f>
-        <v>5.98</v>
-      </c>
-      <c r="E66" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F66" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A67" t="s">
-        <v>59</v>
-      </c>
-      <c r="B67">
-        <v>1</v>
-      </c>
-      <c r="C67" s="16">
-        <v>162.24</v>
-      </c>
-      <c r="D67" s="7">
         <f t="shared" si="7"/>
         <v>162.24</v>
       </c>
-      <c r="E67" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="F67" t="s">
+      <c r="E66" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F66" t="s">
         <v>61</v>
       </c>
     </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B67" s="2"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="8">
+        <f>SUM(D63:D66)</f>
+        <v>248.99</v>
+      </c>
+      <c r="E67" s="5"/>
+    </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A68" s="2" t="s">
-        <v>12</v>
-      </c>
+      <c r="A68" s="2"/>
       <c r="B68" s="2"/>
       <c r="C68" s="8"/>
-      <c r="D68" s="8">
-        <f>SUM(D64:D67)</f>
-        <v>248.99</v>
-      </c>
+      <c r="D68" s="8"/>
       <c r="E68" s="5"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A69" s="2"/>
-      <c r="B69" s="2"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="8"/>
-      <c r="E69" s="5"/>
+      <c r="A69" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B69" s="10"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="13">
+        <f>SUM(D19,D36,D50,D60,D67)</f>
+        <v>4311.62</v>
+      </c>
+      <c r="E69" s="14"/>
+      <c r="F69" s="11"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A70" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B70" s="10"/>
-      <c r="C70" s="13"/>
-      <c r="D70" s="13">
-        <f>SUM(D19,D37,D51,D61,D68)</f>
-        <v>4298.25</v>
-      </c>
-      <c r="E70" s="14"/>
-      <c r="F70" s="11"/>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A71" s="2"/>
-      <c r="B71" s="2"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-      <c r="E71" s="5"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2"/>
+      <c r="A70" s="2"/>
+      <c r="B70" s="2"/>
+      <c r="C70" s="8"/>
+      <c r="D70" s="8"/>
+      <c r="E70" s="5"/>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A75" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{265C8903-4AEC-DE44-B1F0-7DCFD4E09549}"/>
     <hyperlink ref="E6" r:id="rId2" xr:uid="{D7F77966-9390-464E-8627-399015801D2B}"/>
-    <hyperlink ref="E54" r:id="rId3" xr:uid="{753A6B9C-278C-CF4C-84C9-5C0074671CCB}"/>
+    <hyperlink ref="E53" r:id="rId3" xr:uid="{753A6B9C-278C-CF4C-84C9-5C0074671CCB}"/>
     <hyperlink ref="E7" r:id="rId4" xr:uid="{ABA722A5-FBD9-5648-907E-EA5124EDD3C7}"/>
     <hyperlink ref="E4" r:id="rId5" xr:uid="{E86130E0-C24B-4999-BA56-A93018628621}"/>
     <hyperlink ref="E8" r:id="rId6" xr:uid="{5EBE1F0E-BB73-4E1F-930A-245A6D604944}"/>
@@ -2060,44 +2054,46 @@
     <hyperlink ref="E12" r:id="rId9" xr:uid="{50D931CC-3B6E-42C8-808A-560D3BAA8C9B}"/>
     <hyperlink ref="E13" r:id="rId10" xr:uid="{932D3A23-2C68-463E-B52B-0FE8F78ACCDF}"/>
     <hyperlink ref="E23" r:id="rId11" xr:uid="{53B2F0F9-A580-4861-BD66-85ABAE1CCBAE}"/>
-    <hyperlink ref="E55" r:id="rId12" xr:uid="{FFFB96A5-D75D-44BD-A842-0A4287651080}"/>
-    <hyperlink ref="E59" r:id="rId13" xr:uid="{F23935C7-47F1-4B40-BADF-D879792EF9DE}"/>
-    <hyperlink ref="E57" r:id="rId14" xr:uid="{1D128B7C-5EF3-484D-8C28-188F278102B0}"/>
-    <hyperlink ref="E58" r:id="rId15" xr:uid="{3D0664EC-1A4C-4C99-B561-BD442A1E3D41}"/>
-    <hyperlink ref="E67" r:id="rId16" xr:uid="{B7BD41D6-7DEE-43DB-95AF-95E2AAD32A07}"/>
-    <hyperlink ref="E29" r:id="rId17" xr:uid="{4584B495-BC8B-4A56-8488-938C8F973486}"/>
-    <hyperlink ref="E31" r:id="rId18" xr:uid="{4CFD3088-B3B3-4D6F-871E-6C39CB72D32C}"/>
-    <hyperlink ref="E36" r:id="rId19" xr:uid="{6F13B64E-341D-4630-9A15-274D20E0D01A}"/>
-    <hyperlink ref="E32" r:id="rId20" xr:uid="{D339FF2C-D50A-4B5C-95DB-4E5B1D2FC78C}"/>
+    <hyperlink ref="E54" r:id="rId12" xr:uid="{FFFB96A5-D75D-44BD-A842-0A4287651080}"/>
+    <hyperlink ref="E58" r:id="rId13" xr:uid="{F23935C7-47F1-4B40-BADF-D879792EF9DE}"/>
+    <hyperlink ref="E56" r:id="rId14" xr:uid="{1D128B7C-5EF3-484D-8C28-188F278102B0}"/>
+    <hyperlink ref="E57" r:id="rId15" xr:uid="{3D0664EC-1A4C-4C99-B561-BD442A1E3D41}"/>
+    <hyperlink ref="E66" r:id="rId16" xr:uid="{B7BD41D6-7DEE-43DB-95AF-95E2AAD32A07}"/>
+    <hyperlink ref="E28" r:id="rId17" xr:uid="{4584B495-BC8B-4A56-8488-938C8F973486}"/>
+    <hyperlink ref="E30" r:id="rId18" xr:uid="{4CFD3088-B3B3-4D6F-871E-6C39CB72D32C}"/>
+    <hyperlink ref="E35" r:id="rId19" xr:uid="{6F13B64E-341D-4630-9A15-274D20E0D01A}"/>
+    <hyperlink ref="E31" r:id="rId20" xr:uid="{D339FF2C-D50A-4B5C-95DB-4E5B1D2FC78C}"/>
     <hyperlink ref="E14" r:id="rId21" xr:uid="{AA0AA21E-916F-4519-ACCE-D922984B922D}"/>
     <hyperlink ref="E15" r:id="rId22" xr:uid="{2B688FC6-3D9D-41FE-A949-09240AFE614E}"/>
     <hyperlink ref="E18" r:id="rId23" xr:uid="{2B9323DA-1AF6-4F75-A730-CBCDA0051360}"/>
     <hyperlink ref="E16" r:id="rId24" xr:uid="{522CDC08-C296-4B19-AF41-6EE0D735451A}"/>
     <hyperlink ref="E17" r:id="rId25" xr:uid="{E2623B61-A04B-4912-8A60-A55C2FA9936D}"/>
-    <hyperlink ref="E34" r:id="rId26" xr:uid="{319EF437-6976-40FE-A61A-7768248D5FF7}"/>
-    <hyperlink ref="E35" r:id="rId27" xr:uid="{DECD7A00-C6E8-47A8-933C-60A59B1E6C6D}"/>
-    <hyperlink ref="E56" r:id="rId28" xr:uid="{B32FBE35-C99A-5D4E-BADE-D0C8CE13F03D}"/>
-    <hyperlink ref="E40" r:id="rId29" xr:uid="{9520AE20-32D8-42A4-AC8A-6B9E09D13355}"/>
-    <hyperlink ref="E46" r:id="rId30" xr:uid="{AC8F8736-A208-419B-856C-45013BE07EF7}"/>
-    <hyperlink ref="E33" r:id="rId31" xr:uid="{114F8B26-2853-411C-BCF7-B0909C619271}"/>
-    <hyperlink ref="E41" r:id="rId32" xr:uid="{E3F174FE-8B60-4142-B932-3C44723A0AA1}"/>
-    <hyperlink ref="E45" r:id="rId33" xr:uid="{D087EFAF-53DA-4B2B-AAA1-FF91250773BD}"/>
-    <hyperlink ref="E60" r:id="rId34" xr:uid="{5CE36F16-32E6-4943-8366-5E64B2070BBC}"/>
-    <hyperlink ref="E64" r:id="rId35" xr:uid="{8E9ED613-F7A0-4100-ADC8-368FDA17CD57}"/>
-    <hyperlink ref="E66" r:id="rId36" xr:uid="{179293DB-DDD9-476F-A2B7-DA952B7B6F9B}"/>
-    <hyperlink ref="E65" r:id="rId37" xr:uid="{B473FFEF-9E94-4780-ABCB-8611E45CEAE4}"/>
+    <hyperlink ref="E33" r:id="rId26" xr:uid="{319EF437-6976-40FE-A61A-7768248D5FF7}"/>
+    <hyperlink ref="E34" r:id="rId27" xr:uid="{DECD7A00-C6E8-47A8-933C-60A59B1E6C6D}"/>
+    <hyperlink ref="E55" r:id="rId28" xr:uid="{B32FBE35-C99A-5D4E-BADE-D0C8CE13F03D}"/>
+    <hyperlink ref="E39" r:id="rId29" xr:uid="{9520AE20-32D8-42A4-AC8A-6B9E09D13355}"/>
+    <hyperlink ref="E45" r:id="rId30" xr:uid="{AC8F8736-A208-419B-856C-45013BE07EF7}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{114F8B26-2853-411C-BCF7-B0909C619271}"/>
+    <hyperlink ref="E40" r:id="rId32" xr:uid="{E3F174FE-8B60-4142-B932-3C44723A0AA1}"/>
+    <hyperlink ref="E44" r:id="rId33" xr:uid="{D087EFAF-53DA-4B2B-AAA1-FF91250773BD}"/>
+    <hyperlink ref="E59" r:id="rId34" xr:uid="{5CE36F16-32E6-4943-8366-5E64B2070BBC}"/>
+    <hyperlink ref="E63" r:id="rId35" xr:uid="{8E9ED613-F7A0-4100-ADC8-368FDA17CD57}"/>
+    <hyperlink ref="E65" r:id="rId36" xr:uid="{179293DB-DDD9-476F-A2B7-DA952B7B6F9B}"/>
+    <hyperlink ref="E64" r:id="rId37" xr:uid="{B473FFEF-9E94-4780-ABCB-8611E45CEAE4}"/>
     <hyperlink ref="E22" r:id="rId38" xr:uid="{7D969FF4-FE87-4EED-803D-D6946D18E6D9}"/>
     <hyperlink ref="E10" r:id="rId39" xr:uid="{511B1DEF-7A64-4F56-B5C3-A9B56E8A38F1}"/>
-    <hyperlink ref="E30" r:id="rId40" xr:uid="{FC800152-0A9F-48FB-A860-19897B85CFC7}"/>
-    <hyperlink ref="E50" r:id="rId41" xr:uid="{8EF6BB30-AAB1-45D1-96F2-411336844F6F}"/>
-    <hyperlink ref="E42" r:id="rId42" xr:uid="{F162F5DD-ECF6-4AAD-82A0-5CEB7A62744C}"/>
-    <hyperlink ref="E48" r:id="rId43" xr:uid="{3E6F559F-DB1C-437F-ADBE-1770E5607C44}"/>
-    <hyperlink ref="E47" r:id="rId44" xr:uid="{4B6C3B3A-8D07-4F17-B55A-CFE108E53DE5}"/>
-    <hyperlink ref="E49" r:id="rId45" xr:uid="{6F95830A-E3AC-4BAE-B614-16158D3B155A}"/>
-    <hyperlink ref="E43" r:id="rId46" xr:uid="{51769FCC-2B31-438C-93CF-5E35AECD510D}"/>
+    <hyperlink ref="E29" r:id="rId40" xr:uid="{FC800152-0A9F-48FB-A860-19897B85CFC7}"/>
+    <hyperlink ref="E49" r:id="rId41" xr:uid="{8EF6BB30-AAB1-45D1-96F2-411336844F6F}"/>
+    <hyperlink ref="E41" r:id="rId42" xr:uid="{F162F5DD-ECF6-4AAD-82A0-5CEB7A62744C}"/>
+    <hyperlink ref="E47" r:id="rId43" xr:uid="{3E6F559F-DB1C-437F-ADBE-1770E5607C44}"/>
+    <hyperlink ref="E46" r:id="rId44" xr:uid="{4B6C3B3A-8D07-4F17-B55A-CFE108E53DE5}"/>
+    <hyperlink ref="E48" r:id="rId45" xr:uid="{6F95830A-E3AC-4BAE-B614-16158D3B155A}"/>
+    <hyperlink ref="E42" r:id="rId46" xr:uid="{51769FCC-2B31-438C-93CF-5E35AECD510D}"/>
     <hyperlink ref="E24" r:id="rId47" xr:uid="{51B9F6A1-44F1-47A4-9472-146EE87C4544}"/>
     <hyperlink ref="E25" r:id="rId48" xr:uid="{CF4C9E98-B627-4ACE-8859-F837D6A6E6AC}"/>
-    <hyperlink ref="E44" r:id="rId49" xr:uid="{68F23187-5D62-45AE-8C50-D9F3C163E618}"/>
+    <hyperlink ref="E43" r:id="rId49" xr:uid="{68F23187-5D62-45AE-8C50-D9F3C163E618}"/>
+    <hyperlink ref="E27" r:id="rId50" xr:uid="{0D8AEB66-0831-4EF1-B4A7-B6F6F23ECC83}"/>
+    <hyperlink ref="E26" r:id="rId51" xr:uid="{0AA8DA14-283A-4C3A-A977-E8406BF73086}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added photos for guides and adjusted the price of the Solperk solar panel and charge controller on the cost spreadsheet
</commit_message>
<xml_diff>
--- a/hardware/hardware_spreadsheet_not_campbellsci.xlsx
+++ b/hardware/hardware_spreadsheet_not_campbellsci.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Braedon Dority\Documents\GitHub\snow_sensing\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F046F050-452D-49BC-96F6-403E5899D934}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA3C6C0-81C5-424C-911A-5FD543142748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15264" yWindow="0" windowWidth="15552" windowHeight="16656" xr2:uid="{6EB52CEB-1D4B-9D4B-8914-58F1C62D238A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{6EB52CEB-1D4B-9D4B-8914-58F1C62D238A}"/>
   </bookViews>
   <sheets>
     <sheet name="Low-Cost Snow Station" sheetId="2" r:id="rId1"/>
@@ -837,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D4E0150-E134-1049-A012-C7D00DAA06DE}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B65" sqref="B65"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1564,11 +1564,11 @@
         <v>1</v>
       </c>
       <c r="C41" s="7">
-        <v>74.989999999999995</v>
+        <v>54</v>
       </c>
       <c r="D41" s="7">
         <f t="shared" ref="D41:D44" si="5">B41*C41</f>
-        <v>74.989999999999995</v>
+        <v>54</v>
       </c>
       <c r="E41" s="4" t="s">
         <v>16</v>
@@ -1690,7 +1690,7 @@
       <c r="C47" s="8"/>
       <c r="D47" s="8">
         <f>SUM(D40:D46)</f>
-        <v>208.24</v>
+        <v>187.25</v>
       </c>
       <c r="E47" s="5"/>
     </row>
@@ -2038,7 +2038,7 @@
       <c r="C69" s="13"/>
       <c r="D69" s="13">
         <f>SUM(D20,D37,D47,D56,D67)</f>
-        <v>4163.1000000000004</v>
+        <v>4142.1099999999997</v>
       </c>
       <c r="E69" s="14"/>
       <c r="F69" s="11"/>

</xml_diff>